<commit_message>
[SAU-1563] combine ices div and subdiv
</commit_message>
<xml_diff>
--- a/test_uploads/new_test_data.xlsx
+++ b/test_uploads/new_test_data.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="34">
   <si>
     <t>fishing entity</t>
   </si>
@@ -35,10 +35,7 @@
     <t>province state</t>
   </si>
   <si>
-    <t>ICES division</t>
-  </si>
-  <si>
-    <t>ICES subdivision</t>
+    <t>ICES area</t>
   </si>
   <si>
     <t>NAFO division</t>
@@ -1544,7 +1541,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AB20"/>
+  <dimension ref="A1:AA20"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1577,8 +1574,7 @@
     <col min="25" max="25" width="9.125" style="1" customWidth="1"/>
     <col min="26" max="26" width="9.125" style="1" customWidth="1"/>
     <col min="27" max="27" width="9.125" style="1" customWidth="1"/>
-    <col min="28" max="28" width="9.125" style="1" customWidth="1"/>
-    <col min="29" max="256" width="9" style="1" customWidth="1"/>
+    <col min="28" max="256" width="9" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="15" customHeight="1">
@@ -1660,11 +1656,8 @@
       <c r="Z1" t="s" s="3">
         <v>25</v>
       </c>
-      <c r="AA1" t="s" s="3">
+      <c r="AA1" t="s" s="4">
         <v>26</v>
-      </c>
-      <c r="AB1" t="s" s="4">
-        <v>27</v>
       </c>
     </row>
     <row r="2" ht="20.15" customHeight="1">
@@ -1684,9 +1677,11 @@
       <c r="H2" s="6"/>
       <c r="I2" s="6"/>
       <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
-      <c r="L2" s="5">
+      <c r="K2" s="5">
         <v>2</v>
+      </c>
+      <c r="L2" t="s" s="5">
+        <v>27</v>
       </c>
       <c r="M2" t="s" s="5">
         <v>28</v>
@@ -1694,33 +1689,30 @@
       <c r="N2" t="s" s="5">
         <v>29</v>
       </c>
-      <c r="O2" t="s" s="5">
+      <c r="O2" s="5">
+        <v>1951</v>
+      </c>
+      <c r="P2" t="s" s="5">
         <v>30</v>
       </c>
-      <c r="P2" s="5">
-        <v>1951</v>
-      </c>
-      <c r="Q2" t="s" s="5">
+      <c r="Q2" s="6"/>
+      <c r="R2" s="6"/>
+      <c r="S2" s="5">
+        <v>12.8212595279804</v>
+      </c>
+      <c r="T2" s="6"/>
+      <c r="U2" s="6"/>
+      <c r="V2" t="s" s="5">
         <v>31</v>
       </c>
-      <c r="R2" s="6"/>
-      <c r="S2" s="6"/>
-      <c r="T2" s="5">
-        <v>12.8212595279804</v>
-      </c>
-      <c r="U2" s="6"/>
-      <c r="V2" s="6"/>
-      <c r="W2" t="s" s="5">
-        <v>32</v>
-      </c>
+      <c r="W2" s="6"/>
       <c r="X2" s="6"/>
       <c r="Y2" s="6"/>
-      <c r="Z2" s="6"/>
-      <c r="AA2" s="5">
+      <c r="Z2" s="5">
         <v>167</v>
       </c>
-      <c r="AB2" t="s" s="5">
-        <v>33</v>
+      <c r="AA2" t="s" s="5">
+        <v>32</v>
       </c>
     </row>
     <row r="3" ht="20.35" customHeight="1">
@@ -1740,9 +1732,11 @@
       <c r="H3" s="8"/>
       <c r="I3" s="8"/>
       <c r="J3" s="8"/>
-      <c r="K3" s="8"/>
-      <c r="L3" s="7">
+      <c r="K3" s="7">
         <v>2</v>
+      </c>
+      <c r="L3" t="s" s="7">
+        <v>27</v>
       </c>
       <c r="M3" t="s" s="7">
         <v>28</v>
@@ -1750,33 +1744,30 @@
       <c r="N3" t="s" s="7">
         <v>29</v>
       </c>
-      <c r="O3" t="s" s="7">
+      <c r="O3" s="7">
+        <v>1951</v>
+      </c>
+      <c r="P3" t="s" s="7">
         <v>30</v>
       </c>
-      <c r="P3" s="7">
-        <v>1951</v>
-      </c>
-      <c r="Q3" t="s" s="7">
+      <c r="Q3" s="8"/>
+      <c r="R3" s="8"/>
+      <c r="S3" s="7">
+        <v>7.23909255914716</v>
+      </c>
+      <c r="T3" s="8"/>
+      <c r="U3" s="8"/>
+      <c r="V3" t="s" s="7">
         <v>31</v>
       </c>
-      <c r="R3" s="8"/>
-      <c r="S3" s="8"/>
-      <c r="T3" s="7">
-        <v>7.23909255914716</v>
-      </c>
-      <c r="U3" s="8"/>
-      <c r="V3" s="8"/>
-      <c r="W3" t="s" s="7">
-        <v>32</v>
-      </c>
+      <c r="W3" s="8"/>
       <c r="X3" s="8"/>
       <c r="Y3" s="8"/>
-      <c r="Z3" s="8"/>
-      <c r="AA3" s="7">
+      <c r="Z3" s="7">
         <v>167</v>
       </c>
-      <c r="AB3" t="s" s="7">
-        <v>34</v>
+      <c r="AA3" t="s" s="7">
+        <v>33</v>
       </c>
     </row>
     <row r="4" ht="20.35" customHeight="1">
@@ -1796,9 +1787,11 @@
       <c r="H4" s="8"/>
       <c r="I4" s="8"/>
       <c r="J4" s="8"/>
-      <c r="K4" s="8"/>
-      <c r="L4" s="7">
+      <c r="K4" s="7">
         <v>2</v>
+      </c>
+      <c r="L4" t="s" s="7">
+        <v>27</v>
       </c>
       <c r="M4" t="s" s="7">
         <v>28</v>
@@ -1806,33 +1799,30 @@
       <c r="N4" t="s" s="7">
         <v>29</v>
       </c>
-      <c r="O4" t="s" s="7">
+      <c r="O4" s="7">
+        <v>1952</v>
+      </c>
+      <c r="P4" t="s" s="7">
         <v>30</v>
       </c>
-      <c r="P4" s="7">
-        <v>1952</v>
-      </c>
-      <c r="Q4" t="s" s="7">
+      <c r="Q4" s="8"/>
+      <c r="R4" s="8"/>
+      <c r="S4" s="7">
+        <v>51.140148484989</v>
+      </c>
+      <c r="T4" s="8"/>
+      <c r="U4" s="8"/>
+      <c r="V4" t="s" s="7">
         <v>31</v>
       </c>
-      <c r="R4" s="8"/>
-      <c r="S4" s="8"/>
-      <c r="T4" s="7">
-        <v>51.140148484989</v>
-      </c>
-      <c r="U4" s="8"/>
-      <c r="V4" s="8"/>
-      <c r="W4" t="s" s="7">
-        <v>32</v>
-      </c>
+      <c r="W4" s="8"/>
       <c r="X4" s="8"/>
       <c r="Y4" s="8"/>
-      <c r="Z4" s="8"/>
-      <c r="AA4" s="7">
+      <c r="Z4" s="7">
         <v>167</v>
       </c>
-      <c r="AB4" t="s" s="7">
-        <v>33</v>
+      <c r="AA4" t="s" s="7">
+        <v>32</v>
       </c>
     </row>
     <row r="5" ht="20.35" customHeight="1">
@@ -1852,9 +1842,11 @@
       <c r="H5" s="8"/>
       <c r="I5" s="8"/>
       <c r="J5" s="8"/>
-      <c r="K5" s="8"/>
-      <c r="L5" s="7">
+      <c r="K5" s="7">
         <v>2</v>
+      </c>
+      <c r="L5" t="s" s="7">
+        <v>27</v>
       </c>
       <c r="M5" t="s" s="7">
         <v>28</v>
@@ -1862,33 +1854,30 @@
       <c r="N5" t="s" s="7">
         <v>29</v>
       </c>
-      <c r="O5" t="s" s="7">
+      <c r="O5" s="7">
+        <v>1952</v>
+      </c>
+      <c r="P5" t="s" s="7">
         <v>30</v>
       </c>
-      <c r="P5" s="7">
-        <v>1952</v>
-      </c>
-      <c r="Q5" t="s" s="7">
+      <c r="Q5" s="8"/>
+      <c r="R5" s="8"/>
+      <c r="S5" s="7">
+        <v>14.4781851182943</v>
+      </c>
+      <c r="T5" s="8"/>
+      <c r="U5" s="8"/>
+      <c r="V5" t="s" s="7">
         <v>31</v>
       </c>
-      <c r="R5" s="8"/>
-      <c r="S5" s="8"/>
-      <c r="T5" s="7">
-        <v>14.4781851182943</v>
-      </c>
-      <c r="U5" s="8"/>
-      <c r="V5" s="8"/>
-      <c r="W5" t="s" s="7">
-        <v>32</v>
-      </c>
+      <c r="W5" s="8"/>
       <c r="X5" s="8"/>
       <c r="Y5" s="8"/>
-      <c r="Z5" s="8"/>
-      <c r="AA5" s="7">
+      <c r="Z5" s="7">
         <v>167</v>
       </c>
-      <c r="AB5" t="s" s="7">
-        <v>34</v>
+      <c r="AA5" t="s" s="7">
+        <v>33</v>
       </c>
     </row>
     <row r="6" ht="20.35" customHeight="1">
@@ -1908,9 +1897,11 @@
       <c r="H6" s="8"/>
       <c r="I6" s="8"/>
       <c r="J6" s="8"/>
-      <c r="K6" s="8"/>
-      <c r="L6" s="7">
+      <c r="K6" s="7">
         <v>2</v>
+      </c>
+      <c r="L6" t="s" s="7">
+        <v>27</v>
       </c>
       <c r="M6" t="s" s="7">
         <v>28</v>
@@ -1918,33 +1909,30 @@
       <c r="N6" t="s" s="7">
         <v>29</v>
       </c>
-      <c r="O6" t="s" s="7">
+      <c r="O6" s="7">
+        <v>1953</v>
+      </c>
+      <c r="P6" t="s" s="7">
         <v>30</v>
       </c>
-      <c r="P6" s="7">
-        <v>1953</v>
-      </c>
-      <c r="Q6" t="s" s="7">
+      <c r="Q6" s="8"/>
+      <c r="R6" s="8"/>
+      <c r="S6" s="7">
+        <v>114.736682010622</v>
+      </c>
+      <c r="T6" s="8"/>
+      <c r="U6" s="8"/>
+      <c r="V6" t="s" s="7">
         <v>31</v>
       </c>
-      <c r="R6" s="8"/>
-      <c r="S6" s="8"/>
-      <c r="T6" s="7">
-        <v>114.736682010622</v>
-      </c>
-      <c r="U6" s="8"/>
-      <c r="V6" s="8"/>
-      <c r="W6" t="s" s="7">
-        <v>32</v>
-      </c>
+      <c r="W6" s="8"/>
       <c r="X6" s="8"/>
       <c r="Y6" s="8"/>
-      <c r="Z6" s="8"/>
-      <c r="AA6" s="7">
+      <c r="Z6" s="7">
         <v>167</v>
       </c>
-      <c r="AB6" t="s" s="7">
-        <v>33</v>
+      <c r="AA6" t="s" s="7">
+        <v>32</v>
       </c>
     </row>
     <row r="7" ht="20.35" customHeight="1">
@@ -1964,9 +1952,11 @@
       <c r="H7" s="8"/>
       <c r="I7" s="8"/>
       <c r="J7" s="8"/>
-      <c r="K7" s="8"/>
-      <c r="L7" s="7">
+      <c r="K7" s="7">
         <v>2</v>
+      </c>
+      <c r="L7" t="s" s="7">
+        <v>27</v>
       </c>
       <c r="M7" t="s" s="7">
         <v>28</v>
@@ -1974,33 +1964,30 @@
       <c r="N7" t="s" s="7">
         <v>29</v>
       </c>
-      <c r="O7" t="s" s="7">
+      <c r="O7" s="7">
+        <v>1953</v>
+      </c>
+      <c r="P7" t="s" s="7">
         <v>30</v>
       </c>
-      <c r="P7" s="7">
-        <v>1953</v>
-      </c>
-      <c r="Q7" t="s" s="7">
+      <c r="Q7" s="8"/>
+      <c r="R7" s="8"/>
+      <c r="S7" s="7">
+        <v>21.7172776774415</v>
+      </c>
+      <c r="T7" s="8"/>
+      <c r="U7" s="8"/>
+      <c r="V7" t="s" s="7">
         <v>31</v>
       </c>
-      <c r="R7" s="8"/>
-      <c r="S7" s="8"/>
-      <c r="T7" s="7">
-        <v>21.7172776774415</v>
-      </c>
-      <c r="U7" s="8"/>
-      <c r="V7" s="8"/>
-      <c r="W7" t="s" s="7">
-        <v>32</v>
-      </c>
+      <c r="W7" s="8"/>
       <c r="X7" s="8"/>
       <c r="Y7" s="8"/>
-      <c r="Z7" s="8"/>
-      <c r="AA7" s="7">
+      <c r="Z7" s="7">
         <v>167</v>
       </c>
-      <c r="AB7" t="s" s="7">
-        <v>34</v>
+      <c r="AA7" t="s" s="7">
+        <v>33</v>
       </c>
     </row>
     <row r="8" ht="20.35" customHeight="1">
@@ -2020,9 +2007,11 @@
       <c r="H8" s="8"/>
       <c r="I8" s="8"/>
       <c r="J8" s="8"/>
-      <c r="K8" s="8"/>
-      <c r="L8" s="7">
+      <c r="K8" s="7">
         <v>2</v>
+      </c>
+      <c r="L8" t="s" s="7">
+        <v>27</v>
       </c>
       <c r="M8" t="s" s="7">
         <v>28</v>
@@ -2030,33 +2019,30 @@
       <c r="N8" t="s" s="7">
         <v>29</v>
       </c>
-      <c r="O8" t="s" s="7">
+      <c r="O8" s="7">
+        <v>1954</v>
+      </c>
+      <c r="P8" t="s" s="7">
         <v>30</v>
       </c>
-      <c r="P8" s="7">
-        <v>1954</v>
-      </c>
-      <c r="Q8" t="s" s="7">
+      <c r="Q8" s="8"/>
+      <c r="R8" s="8"/>
+      <c r="S8" s="7">
+        <v>203.387341351136</v>
+      </c>
+      <c r="T8" s="8"/>
+      <c r="U8" s="8"/>
+      <c r="V8" t="s" s="7">
         <v>31</v>
       </c>
-      <c r="R8" s="8"/>
-      <c r="S8" s="8"/>
-      <c r="T8" s="7">
-        <v>203.387341351136</v>
-      </c>
-      <c r="U8" s="8"/>
-      <c r="V8" s="8"/>
-      <c r="W8" t="s" s="7">
-        <v>32</v>
-      </c>
+      <c r="W8" s="8"/>
       <c r="X8" s="8"/>
       <c r="Y8" s="8"/>
-      <c r="Z8" s="8"/>
-      <c r="AA8" s="7">
+      <c r="Z8" s="7">
         <v>167</v>
       </c>
-      <c r="AB8" t="s" s="7">
-        <v>33</v>
+      <c r="AA8" t="s" s="7">
+        <v>32</v>
       </c>
     </row>
     <row r="9" ht="20.35" customHeight="1">
@@ -2076,9 +2062,11 @@
       <c r="H9" s="8"/>
       <c r="I9" s="8"/>
       <c r="J9" s="8"/>
-      <c r="K9" s="8"/>
-      <c r="L9" s="7">
+      <c r="K9" s="7">
         <v>2</v>
+      </c>
+      <c r="L9" t="s" s="7">
+        <v>27</v>
       </c>
       <c r="M9" t="s" s="7">
         <v>28</v>
@@ -2086,33 +2074,30 @@
       <c r="N9" t="s" s="7">
         <v>29</v>
       </c>
-      <c r="O9" t="s" s="7">
+      <c r="O9" s="7">
+        <v>1954</v>
+      </c>
+      <c r="P9" t="s" s="7">
         <v>30</v>
       </c>
-      <c r="P9" s="7">
-        <v>1954</v>
-      </c>
-      <c r="Q9" t="s" s="7">
+      <c r="Q9" s="8"/>
+      <c r="R9" s="8"/>
+      <c r="S9" s="7">
+        <v>28.9563702365887</v>
+      </c>
+      <c r="T9" s="8"/>
+      <c r="U9" s="8"/>
+      <c r="V9" t="s" s="7">
         <v>31</v>
       </c>
-      <c r="R9" s="8"/>
-      <c r="S9" s="8"/>
-      <c r="T9" s="7">
-        <v>28.9563702365887</v>
-      </c>
-      <c r="U9" s="8"/>
-      <c r="V9" s="8"/>
-      <c r="W9" t="s" s="7">
-        <v>32</v>
-      </c>
+      <c r="W9" s="8"/>
       <c r="X9" s="8"/>
       <c r="Y9" s="8"/>
-      <c r="Z9" s="8"/>
-      <c r="AA9" s="7">
+      <c r="Z9" s="7">
         <v>167</v>
       </c>
-      <c r="AB9" t="s" s="7">
-        <v>34</v>
+      <c r="AA9" t="s" s="7">
+        <v>33</v>
       </c>
     </row>
     <row r="10" ht="20.35" customHeight="1">
@@ -2132,9 +2117,11 @@
       <c r="H10" s="8"/>
       <c r="I10" s="8"/>
       <c r="J10" s="8"/>
-      <c r="K10" s="8"/>
-      <c r="L10" s="7">
+      <c r="K10" s="7">
         <v>2</v>
+      </c>
+      <c r="L10" t="s" s="7">
+        <v>27</v>
       </c>
       <c r="M10" t="s" s="7">
         <v>28</v>
@@ -2142,33 +2129,30 @@
       <c r="N10" t="s" s="7">
         <v>29</v>
       </c>
-      <c r="O10" t="s" s="7">
+      <c r="O10" s="7">
+        <v>1955</v>
+      </c>
+      <c r="P10" t="s" s="7">
         <v>30</v>
       </c>
-      <c r="P10" s="7">
-        <v>1955</v>
-      </c>
-      <c r="Q10" t="s" s="7">
+      <c r="Q10" s="8"/>
+      <c r="R10" s="8"/>
+      <c r="S10" s="7">
+        <v>316.865073859446</v>
+      </c>
+      <c r="T10" s="8"/>
+      <c r="U10" s="8"/>
+      <c r="V10" t="s" s="7">
         <v>31</v>
       </c>
-      <c r="R10" s="8"/>
-      <c r="S10" s="8"/>
-      <c r="T10" s="7">
-        <v>316.865073859446</v>
-      </c>
-      <c r="U10" s="8"/>
-      <c r="V10" s="8"/>
-      <c r="W10" t="s" s="7">
-        <v>32</v>
-      </c>
+      <c r="W10" s="8"/>
       <c r="X10" s="8"/>
       <c r="Y10" s="8"/>
-      <c r="Z10" s="8"/>
-      <c r="AA10" s="7">
+      <c r="Z10" s="7">
         <v>167</v>
       </c>
-      <c r="AB10" t="s" s="7">
-        <v>33</v>
+      <c r="AA10" t="s" s="7">
+        <v>32</v>
       </c>
     </row>
     <row r="11" ht="20.35" customHeight="1">
@@ -2199,7 +2183,6 @@
       <c r="Y11" s="8"/>
       <c r="Z11" s="8"/>
       <c r="AA11" s="8"/>
-      <c r="AB11" s="8"/>
     </row>
     <row r="12" ht="20.35" customHeight="1">
       <c r="A12" s="9"/>
@@ -2229,7 +2212,6 @@
       <c r="Y12" s="8"/>
       <c r="Z12" s="8"/>
       <c r="AA12" s="8"/>
-      <c r="AB12" s="8"/>
     </row>
     <row r="13" ht="20.35" customHeight="1">
       <c r="A13" s="9"/>
@@ -2259,7 +2241,6 @@
       <c r="Y13" s="8"/>
       <c r="Z13" s="8"/>
       <c r="AA13" s="8"/>
-      <c r="AB13" s="8"/>
     </row>
     <row r="14" ht="20.35" customHeight="1">
       <c r="A14" s="9"/>
@@ -2289,7 +2270,6 @@
       <c r="Y14" s="8"/>
       <c r="Z14" s="8"/>
       <c r="AA14" s="8"/>
-      <c r="AB14" s="8"/>
     </row>
     <row r="15" ht="20.35" customHeight="1">
       <c r="A15" s="9"/>
@@ -2319,7 +2299,6 @@
       <c r="Y15" s="8"/>
       <c r="Z15" s="8"/>
       <c r="AA15" s="8"/>
-      <c r="AB15" s="8"/>
     </row>
     <row r="16" ht="20.35" customHeight="1">
       <c r="A16" s="9"/>
@@ -2349,7 +2328,6 @@
       <c r="Y16" s="8"/>
       <c r="Z16" s="8"/>
       <c r="AA16" s="8"/>
-      <c r="AB16" s="8"/>
     </row>
     <row r="17" ht="20.35" customHeight="1">
       <c r="A17" s="9"/>
@@ -2379,7 +2357,6 @@
       <c r="Y17" s="8"/>
       <c r="Z17" s="8"/>
       <c r="AA17" s="8"/>
-      <c r="AB17" s="8"/>
     </row>
     <row r="18" ht="20.35" customHeight="1">
       <c r="A18" s="9"/>
@@ -2409,7 +2386,6 @@
       <c r="Y18" s="8"/>
       <c r="Z18" s="8"/>
       <c r="AA18" s="8"/>
-      <c r="AB18" s="8"/>
     </row>
     <row r="19" ht="20.35" customHeight="1">
       <c r="A19" s="9"/>
@@ -2439,7 +2415,6 @@
       <c r="Y19" s="8"/>
       <c r="Z19" s="8"/>
       <c r="AA19" s="8"/>
-      <c r="AB19" s="8"/>
     </row>
     <row r="20" ht="20.35" customHeight="1">
       <c r="A20" s="9"/>
@@ -2469,7 +2444,6 @@
       <c r="Y20" s="8"/>
       <c r="Z20" s="8"/>
       <c r="AA20" s="8"/>
-      <c r="AB20" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
set reference on file upload
</commit_message>
<xml_diff>
--- a/test_uploads/new_test_data.xlsx
+++ b/test_uploads/new_test_data.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="33">
   <si>
     <t>fishing entity</t>
   </si>
@@ -87,9 +87,6 @@
   </si>
   <si>
     <t>layer rule</t>
-  </si>
-  <si>
-    <t>reference id</t>
   </si>
   <si>
     <t>notes</t>
@@ -1541,7 +1538,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AA20"/>
+  <dimension ref="A1:Z20"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1573,8 +1570,7 @@
     <col min="24" max="24" width="9.125" style="1" customWidth="1"/>
     <col min="25" max="25" width="9.125" style="1" customWidth="1"/>
     <col min="26" max="26" width="9.125" style="1" customWidth="1"/>
-    <col min="27" max="27" width="9.125" style="1" customWidth="1"/>
-    <col min="28" max="256" width="9" style="1" customWidth="1"/>
+    <col min="27" max="256" width="9" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="15" customHeight="1">
@@ -1653,11 +1649,8 @@
       <c r="Y1" t="s" s="3">
         <v>24</v>
       </c>
-      <c r="Z1" t="s" s="3">
+      <c r="Z1" t="s" s="4">
         <v>25</v>
-      </c>
-      <c r="AA1" t="s" s="4">
-        <v>26</v>
       </c>
     </row>
     <row r="2" ht="20.15" customHeight="1">
@@ -1681,19 +1674,19 @@
         <v>2</v>
       </c>
       <c r="L2" t="s" s="5">
+        <v>26</v>
+      </c>
+      <c r="M2" t="s" s="5">
         <v>27</v>
       </c>
-      <c r="M2" t="s" s="5">
+      <c r="N2" t="s" s="5">
         <v>28</v>
-      </c>
-      <c r="N2" t="s" s="5">
-        <v>29</v>
       </c>
       <c r="O2" s="5">
         <v>1951</v>
       </c>
       <c r="P2" t="s" s="5">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="Q2" s="6"/>
       <c r="R2" s="6"/>
@@ -1703,16 +1696,13 @@
       <c r="T2" s="6"/>
       <c r="U2" s="6"/>
       <c r="V2" t="s" s="5">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="W2" s="6"/>
       <c r="X2" s="6"/>
       <c r="Y2" s="6"/>
-      <c r="Z2" s="5">
-        <v>167</v>
-      </c>
-      <c r="AA2" t="s" s="5">
-        <v>32</v>
+      <c r="Z2" t="s" s="5">
+        <v>31</v>
       </c>
     </row>
     <row r="3" ht="20.35" customHeight="1">
@@ -1736,19 +1726,19 @@
         <v>2</v>
       </c>
       <c r="L3" t="s" s="7">
+        <v>26</v>
+      </c>
+      <c r="M3" t="s" s="7">
         <v>27</v>
       </c>
-      <c r="M3" t="s" s="7">
+      <c r="N3" t="s" s="7">
         <v>28</v>
-      </c>
-      <c r="N3" t="s" s="7">
-        <v>29</v>
       </c>
       <c r="O3" s="7">
         <v>1951</v>
       </c>
       <c r="P3" t="s" s="7">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="Q3" s="8"/>
       <c r="R3" s="8"/>
@@ -1758,16 +1748,13 @@
       <c r="T3" s="8"/>
       <c r="U3" s="8"/>
       <c r="V3" t="s" s="7">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="W3" s="8"/>
       <c r="X3" s="8"/>
       <c r="Y3" s="8"/>
-      <c r="Z3" s="7">
-        <v>167</v>
-      </c>
-      <c r="AA3" t="s" s="7">
-        <v>33</v>
+      <c r="Z3" t="s" s="7">
+        <v>32</v>
       </c>
     </row>
     <row r="4" ht="20.35" customHeight="1">
@@ -1791,19 +1778,19 @@
         <v>2</v>
       </c>
       <c r="L4" t="s" s="7">
+        <v>26</v>
+      </c>
+      <c r="M4" t="s" s="7">
         <v>27</v>
       </c>
-      <c r="M4" t="s" s="7">
+      <c r="N4" t="s" s="7">
         <v>28</v>
-      </c>
-      <c r="N4" t="s" s="7">
-        <v>29</v>
       </c>
       <c r="O4" s="7">
         <v>1952</v>
       </c>
       <c r="P4" t="s" s="7">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="Q4" s="8"/>
       <c r="R4" s="8"/>
@@ -1813,16 +1800,13 @@
       <c r="T4" s="8"/>
       <c r="U4" s="8"/>
       <c r="V4" t="s" s="7">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="W4" s="8"/>
       <c r="X4" s="8"/>
       <c r="Y4" s="8"/>
-      <c r="Z4" s="7">
-        <v>167</v>
-      </c>
-      <c r="AA4" t="s" s="7">
-        <v>32</v>
+      <c r="Z4" t="s" s="7">
+        <v>31</v>
       </c>
     </row>
     <row r="5" ht="20.35" customHeight="1">
@@ -1846,19 +1830,19 @@
         <v>2</v>
       </c>
       <c r="L5" t="s" s="7">
+        <v>26</v>
+      </c>
+      <c r="M5" t="s" s="7">
         <v>27</v>
       </c>
-      <c r="M5" t="s" s="7">
+      <c r="N5" t="s" s="7">
         <v>28</v>
-      </c>
-      <c r="N5" t="s" s="7">
-        <v>29</v>
       </c>
       <c r="O5" s="7">
         <v>1952</v>
       </c>
       <c r="P5" t="s" s="7">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="Q5" s="8"/>
       <c r="R5" s="8"/>
@@ -1868,16 +1852,13 @@
       <c r="T5" s="8"/>
       <c r="U5" s="8"/>
       <c r="V5" t="s" s="7">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="W5" s="8"/>
       <c r="X5" s="8"/>
       <c r="Y5" s="8"/>
-      <c r="Z5" s="7">
-        <v>167</v>
-      </c>
-      <c r="AA5" t="s" s="7">
-        <v>33</v>
+      <c r="Z5" t="s" s="7">
+        <v>32</v>
       </c>
     </row>
     <row r="6" ht="20.35" customHeight="1">
@@ -1901,19 +1882,19 @@
         <v>2</v>
       </c>
       <c r="L6" t="s" s="7">
+        <v>26</v>
+      </c>
+      <c r="M6" t="s" s="7">
         <v>27</v>
       </c>
-      <c r="M6" t="s" s="7">
+      <c r="N6" t="s" s="7">
         <v>28</v>
-      </c>
-      <c r="N6" t="s" s="7">
-        <v>29</v>
       </c>
       <c r="O6" s="7">
         <v>1953</v>
       </c>
       <c r="P6" t="s" s="7">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="Q6" s="8"/>
       <c r="R6" s="8"/>
@@ -1923,16 +1904,13 @@
       <c r="T6" s="8"/>
       <c r="U6" s="8"/>
       <c r="V6" t="s" s="7">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="W6" s="8"/>
       <c r="X6" s="8"/>
       <c r="Y6" s="8"/>
-      <c r="Z6" s="7">
-        <v>167</v>
-      </c>
-      <c r="AA6" t="s" s="7">
-        <v>32</v>
+      <c r="Z6" t="s" s="7">
+        <v>31</v>
       </c>
     </row>
     <row r="7" ht="20.35" customHeight="1">
@@ -1956,19 +1934,19 @@
         <v>2</v>
       </c>
       <c r="L7" t="s" s="7">
+        <v>26</v>
+      </c>
+      <c r="M7" t="s" s="7">
         <v>27</v>
       </c>
-      <c r="M7" t="s" s="7">
+      <c r="N7" t="s" s="7">
         <v>28</v>
-      </c>
-      <c r="N7" t="s" s="7">
-        <v>29</v>
       </c>
       <c r="O7" s="7">
         <v>1953</v>
       </c>
       <c r="P7" t="s" s="7">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="Q7" s="8"/>
       <c r="R7" s="8"/>
@@ -1978,16 +1956,13 @@
       <c r="T7" s="8"/>
       <c r="U7" s="8"/>
       <c r="V7" t="s" s="7">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="W7" s="8"/>
       <c r="X7" s="8"/>
       <c r="Y7" s="8"/>
-      <c r="Z7" s="7">
-        <v>167</v>
-      </c>
-      <c r="AA7" t="s" s="7">
-        <v>33</v>
+      <c r="Z7" t="s" s="7">
+        <v>32</v>
       </c>
     </row>
     <row r="8" ht="20.35" customHeight="1">
@@ -2011,19 +1986,19 @@
         <v>2</v>
       </c>
       <c r="L8" t="s" s="7">
+        <v>26</v>
+      </c>
+      <c r="M8" t="s" s="7">
         <v>27</v>
       </c>
-      <c r="M8" t="s" s="7">
+      <c r="N8" t="s" s="7">
         <v>28</v>
-      </c>
-      <c r="N8" t="s" s="7">
-        <v>29</v>
       </c>
       <c r="O8" s="7">
         <v>1954</v>
       </c>
       <c r="P8" t="s" s="7">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="Q8" s="8"/>
       <c r="R8" s="8"/>
@@ -2033,16 +2008,13 @@
       <c r="T8" s="8"/>
       <c r="U8" s="8"/>
       <c r="V8" t="s" s="7">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="W8" s="8"/>
       <c r="X8" s="8"/>
       <c r="Y8" s="8"/>
-      <c r="Z8" s="7">
-        <v>167</v>
-      </c>
-      <c r="AA8" t="s" s="7">
-        <v>32</v>
+      <c r="Z8" t="s" s="7">
+        <v>31</v>
       </c>
     </row>
     <row r="9" ht="20.35" customHeight="1">
@@ -2066,19 +2038,19 @@
         <v>2</v>
       </c>
       <c r="L9" t="s" s="7">
+        <v>26</v>
+      </c>
+      <c r="M9" t="s" s="7">
         <v>27</v>
       </c>
-      <c r="M9" t="s" s="7">
+      <c r="N9" t="s" s="7">
         <v>28</v>
-      </c>
-      <c r="N9" t="s" s="7">
-        <v>29</v>
       </c>
       <c r="O9" s="7">
         <v>1954</v>
       </c>
       <c r="P9" t="s" s="7">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="Q9" s="8"/>
       <c r="R9" s="8"/>
@@ -2088,16 +2060,13 @@
       <c r="T9" s="8"/>
       <c r="U9" s="8"/>
       <c r="V9" t="s" s="7">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="W9" s="8"/>
       <c r="X9" s="8"/>
       <c r="Y9" s="8"/>
-      <c r="Z9" s="7">
-        <v>167</v>
-      </c>
-      <c r="AA9" t="s" s="7">
-        <v>33</v>
+      <c r="Z9" t="s" s="7">
+        <v>32</v>
       </c>
     </row>
     <row r="10" ht="20.35" customHeight="1">
@@ -2121,19 +2090,19 @@
         <v>2</v>
       </c>
       <c r="L10" t="s" s="7">
+        <v>26</v>
+      </c>
+      <c r="M10" t="s" s="7">
         <v>27</v>
       </c>
-      <c r="M10" t="s" s="7">
+      <c r="N10" t="s" s="7">
         <v>28</v>
-      </c>
-      <c r="N10" t="s" s="7">
-        <v>29</v>
       </c>
       <c r="O10" s="7">
         <v>1955</v>
       </c>
       <c r="P10" t="s" s="7">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="Q10" s="8"/>
       <c r="R10" s="8"/>
@@ -2143,16 +2112,13 @@
       <c r="T10" s="8"/>
       <c r="U10" s="8"/>
       <c r="V10" t="s" s="7">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="W10" s="8"/>
       <c r="X10" s="8"/>
       <c r="Y10" s="8"/>
-      <c r="Z10" s="7">
-        <v>167</v>
-      </c>
-      <c r="AA10" t="s" s="7">
-        <v>32</v>
+      <c r="Z10" t="s" s="7">
+        <v>31</v>
       </c>
     </row>
     <row r="11" ht="20.35" customHeight="1">
@@ -2182,7 +2148,6 @@
       <c r="X11" s="8"/>
       <c r="Y11" s="8"/>
       <c r="Z11" s="8"/>
-      <c r="AA11" s="8"/>
     </row>
     <row r="12" ht="20.35" customHeight="1">
       <c r="A12" s="9"/>
@@ -2211,7 +2176,6 @@
       <c r="X12" s="8"/>
       <c r="Y12" s="8"/>
       <c r="Z12" s="8"/>
-      <c r="AA12" s="8"/>
     </row>
     <row r="13" ht="20.35" customHeight="1">
       <c r="A13" s="9"/>
@@ -2240,7 +2204,6 @@
       <c r="X13" s="8"/>
       <c r="Y13" s="8"/>
       <c r="Z13" s="8"/>
-      <c r="AA13" s="8"/>
     </row>
     <row r="14" ht="20.35" customHeight="1">
       <c r="A14" s="9"/>
@@ -2269,7 +2232,6 @@
       <c r="X14" s="8"/>
       <c r="Y14" s="8"/>
       <c r="Z14" s="8"/>
-      <c r="AA14" s="8"/>
     </row>
     <row r="15" ht="20.35" customHeight="1">
       <c r="A15" s="9"/>
@@ -2298,7 +2260,6 @@
       <c r="X15" s="8"/>
       <c r="Y15" s="8"/>
       <c r="Z15" s="8"/>
-      <c r="AA15" s="8"/>
     </row>
     <row r="16" ht="20.35" customHeight="1">
       <c r="A16" s="9"/>
@@ -2327,7 +2288,6 @@
       <c r="X16" s="8"/>
       <c r="Y16" s="8"/>
       <c r="Z16" s="8"/>
-      <c r="AA16" s="8"/>
     </row>
     <row r="17" ht="20.35" customHeight="1">
       <c r="A17" s="9"/>
@@ -2356,7 +2316,6 @@
       <c r="X17" s="8"/>
       <c r="Y17" s="8"/>
       <c r="Z17" s="8"/>
-      <c r="AA17" s="8"/>
     </row>
     <row r="18" ht="20.35" customHeight="1">
       <c r="A18" s="9"/>
@@ -2385,7 +2344,6 @@
       <c r="X18" s="8"/>
       <c r="Y18" s="8"/>
       <c r="Z18" s="8"/>
-      <c r="AA18" s="8"/>
     </row>
     <row r="19" ht="20.35" customHeight="1">
       <c r="A19" s="9"/>
@@ -2414,7 +2372,6 @@
       <c r="X19" s="8"/>
       <c r="Y19" s="8"/>
       <c r="Z19" s="8"/>
-      <c r="AA19" s="8"/>
     </row>
     <row r="20" ht="20.35" customHeight="1">
       <c r="A20" s="9"/>
@@ -2443,7 +2400,6 @@
       <c r="X20" s="8"/>
       <c r="Y20" s="8"/>
       <c r="Z20" s="8"/>
-      <c r="AA20" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
[LP-25459724] move Province/NAFO/ICES to end of table
</commit_message>
<xml_diff>
--- a/test_uploads/new_test_data.xlsx
+++ b/test_uploads/new_test_data.xlsx
@@ -35,6 +35,54 @@
     <t>province state</t>
   </si>
   <si>
+    <t>layer</t>
+  </si>
+  <si>
+    <t>sector</t>
+  </si>
+  <si>
+    <t>original sector</t>
+  </si>
+  <si>
+    <t>catch type</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>taxon name</t>
+  </si>
+  <si>
+    <t>original taxon name</t>
+  </si>
+  <si>
+    <t>original FAO name</t>
+  </si>
+  <si>
+    <t>amount</t>
+  </si>
+  <si>
+    <t>adjustment factor</t>
+  </si>
+  <si>
+    <t>gear type</t>
+  </si>
+  <si>
+    <t>input type</t>
+  </si>
+  <si>
+    <t>forward carry rule</t>
+  </si>
+  <si>
+    <t>disaggregation rule</t>
+  </si>
+  <si>
+    <t>layer rule</t>
+  </si>
+  <si>
+    <t>notes</t>
+  </si>
+  <si>
     <t>ICES area</t>
   </si>
   <si>
@@ -42,54 +90,6 @@
   </si>
   <si>
     <t>CCAMLR area</t>
-  </si>
-  <si>
-    <t>layer</t>
-  </si>
-  <si>
-    <t>sector</t>
-  </si>
-  <si>
-    <t>original sector</t>
-  </si>
-  <si>
-    <t>catch type</t>
-  </si>
-  <si>
-    <t>year</t>
-  </si>
-  <si>
-    <t>taxon name</t>
-  </si>
-  <si>
-    <t>original taxon name</t>
-  </si>
-  <si>
-    <t>original FAO name</t>
-  </si>
-  <si>
-    <t>amount</t>
-  </si>
-  <si>
-    <t>adjustment factor</t>
-  </si>
-  <si>
-    <t>gear type</t>
-  </si>
-  <si>
-    <t>input type</t>
-  </si>
-  <si>
-    <t>forward carry rule</t>
-  </si>
-  <si>
-    <t>disaggregation rule</t>
-  </si>
-  <si>
-    <t>layer rule</t>
-  </si>
-  <si>
-    <t>notes</t>
   </si>
   <si>
     <t>Industrial</t>
@@ -183,7 +183,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -213,6 +213,19 @@
     </border>
     <border>
       <left/>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
       <right style="thin">
         <color indexed="10"/>
       </right>
@@ -256,7 +269,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -272,11 +285,8 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="1" fontId="6" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
@@ -284,7 +294,19 @@
     <xf numFmtId="1" fontId="6" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="7" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="1" fontId="5" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="3" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1640,766 +1662,766 @@
       <c r="V1" t="s" s="3">
         <v>21</v>
       </c>
-      <c r="W1" t="s" s="3">
+      <c r="W1" t="s" s="4">
         <v>22</v>
       </c>
-      <c r="X1" t="s" s="3">
+      <c r="X1" t="s" s="5">
         <v>23</v>
       </c>
-      <c r="Y1" t="s" s="3">
+      <c r="Y1" t="s" s="5">
         <v>24</v>
       </c>
-      <c r="Z1" t="s" s="4">
+      <c r="Z1" t="s" s="5">
         <v>25</v>
       </c>
     </row>
     <row r="2" ht="20.15" customHeight="1">
-      <c r="A2" s="5">
+      <c r="A2" s="6">
         <v>165</v>
       </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="5">
+      <c r="B2" s="7"/>
+      <c r="C2" s="6">
         <v>686</v>
       </c>
-      <c r="D2" s="6"/>
-      <c r="E2" s="5">
+      <c r="D2" s="7"/>
+      <c r="E2" s="6">
         <v>34</v>
       </c>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="5">
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="6">
         <v>2</v>
       </c>
-      <c r="L2" t="s" s="5">
+      <c r="I2" t="s" s="6">
         <v>26</v>
       </c>
-      <c r="M2" t="s" s="5">
+      <c r="J2" t="s" s="6">
         <v>27</v>
       </c>
-      <c r="N2" t="s" s="5">
+      <c r="K2" t="s" s="6">
         <v>28</v>
       </c>
-      <c r="O2" s="5">
+      <c r="L2" s="6">
         <v>1951</v>
       </c>
-      <c r="P2" t="s" s="5">
+      <c r="M2" t="s" s="6">
         <v>29</v>
       </c>
-      <c r="Q2" s="6"/>
-      <c r="R2" s="6"/>
-      <c r="S2" s="5">
+      <c r="N2" s="7"/>
+      <c r="O2" s="7"/>
+      <c r="P2" s="6">
         <v>12.8212595279804</v>
       </c>
-      <c r="T2" s="6"/>
-      <c r="U2" s="6"/>
-      <c r="V2" t="s" s="5">
+      <c r="Q2" s="7"/>
+      <c r="R2" s="7"/>
+      <c r="S2" t="s" s="6">
         <v>30</v>
       </c>
-      <c r="W2" s="6"/>
-      <c r="X2" s="6"/>
-      <c r="Y2" s="6"/>
-      <c r="Z2" t="s" s="5">
+      <c r="T2" s="7"/>
+      <c r="U2" s="7"/>
+      <c r="V2" s="7"/>
+      <c r="W2" t="s" s="6">
         <v>31</v>
       </c>
+      <c r="X2" s="8"/>
+      <c r="Y2" s="8"/>
+      <c r="Z2" s="8"/>
     </row>
     <row r="3" ht="20.35" customHeight="1">
-      <c r="A3" s="7">
+      <c r="A3" s="9">
         <v>165</v>
       </c>
-      <c r="B3" s="8"/>
-      <c r="C3" s="7">
+      <c r="B3" s="10"/>
+      <c r="C3" s="9">
         <v>686</v>
       </c>
-      <c r="D3" s="8"/>
-      <c r="E3" s="7">
+      <c r="D3" s="10"/>
+      <c r="E3" s="9">
         <v>34</v>
       </c>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
-      <c r="K3" s="7">
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="9">
         <v>2</v>
       </c>
-      <c r="L3" t="s" s="7">
+      <c r="I3" t="s" s="9">
         <v>26</v>
       </c>
-      <c r="M3" t="s" s="7">
+      <c r="J3" t="s" s="9">
         <v>27</v>
       </c>
-      <c r="N3" t="s" s="7">
+      <c r="K3" t="s" s="9">
         <v>28</v>
       </c>
-      <c r="O3" s="7">
+      <c r="L3" s="9">
         <v>1951</v>
       </c>
-      <c r="P3" t="s" s="7">
+      <c r="M3" t="s" s="9">
         <v>29</v>
       </c>
-      <c r="Q3" s="8"/>
-      <c r="R3" s="8"/>
-      <c r="S3" s="7">
+      <c r="N3" s="10"/>
+      <c r="O3" s="10"/>
+      <c r="P3" s="9">
         <v>7.23909255914716</v>
       </c>
-      <c r="T3" s="8"/>
-      <c r="U3" s="8"/>
-      <c r="V3" t="s" s="7">
+      <c r="Q3" s="10"/>
+      <c r="R3" s="10"/>
+      <c r="S3" t="s" s="9">
         <v>30</v>
       </c>
-      <c r="W3" s="8"/>
-      <c r="X3" s="8"/>
-      <c r="Y3" s="8"/>
-      <c r="Z3" t="s" s="7">
+      <c r="T3" s="10"/>
+      <c r="U3" s="10"/>
+      <c r="V3" s="10"/>
+      <c r="W3" t="s" s="9">
         <v>32</v>
       </c>
+      <c r="X3" s="11"/>
+      <c r="Y3" s="11"/>
+      <c r="Z3" s="11"/>
     </row>
     <row r="4" ht="20.35" customHeight="1">
-      <c r="A4" s="7">
+      <c r="A4" s="9">
         <v>165</v>
       </c>
-      <c r="B4" s="8"/>
-      <c r="C4" s="7">
+      <c r="B4" s="10"/>
+      <c r="C4" s="9">
         <v>686</v>
       </c>
-      <c r="D4" s="8"/>
-      <c r="E4" s="7">
+      <c r="D4" s="10"/>
+      <c r="E4" s="9">
         <v>34</v>
       </c>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="8"/>
-      <c r="I4" s="8"/>
-      <c r="J4" s="8"/>
-      <c r="K4" s="7">
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="9">
         <v>2</v>
       </c>
-      <c r="L4" t="s" s="7">
+      <c r="I4" t="s" s="9">
         <v>26</v>
       </c>
-      <c r="M4" t="s" s="7">
+      <c r="J4" t="s" s="9">
         <v>27</v>
       </c>
-      <c r="N4" t="s" s="7">
+      <c r="K4" t="s" s="9">
         <v>28</v>
       </c>
-      <c r="O4" s="7">
+      <c r="L4" s="9">
         <v>1952</v>
       </c>
-      <c r="P4" t="s" s="7">
+      <c r="M4" t="s" s="9">
         <v>29</v>
       </c>
-      <c r="Q4" s="8"/>
-      <c r="R4" s="8"/>
-      <c r="S4" s="7">
+      <c r="N4" s="10"/>
+      <c r="O4" s="10"/>
+      <c r="P4" s="9">
         <v>51.140148484989</v>
       </c>
-      <c r="T4" s="8"/>
-      <c r="U4" s="8"/>
-      <c r="V4" t="s" s="7">
+      <c r="Q4" s="10"/>
+      <c r="R4" s="10"/>
+      <c r="S4" t="s" s="9">
         <v>30</v>
       </c>
-      <c r="W4" s="8"/>
-      <c r="X4" s="8"/>
-      <c r="Y4" s="8"/>
-      <c r="Z4" t="s" s="7">
+      <c r="T4" s="10"/>
+      <c r="U4" s="10"/>
+      <c r="V4" s="10"/>
+      <c r="W4" t="s" s="9">
         <v>31</v>
       </c>
+      <c r="X4" s="11"/>
+      <c r="Y4" s="11"/>
+      <c r="Z4" s="11"/>
     </row>
     <row r="5" ht="20.35" customHeight="1">
-      <c r="A5" s="7">
+      <c r="A5" s="9">
         <v>165</v>
       </c>
-      <c r="B5" s="8"/>
-      <c r="C5" s="7">
+      <c r="B5" s="10"/>
+      <c r="C5" s="9">
         <v>686</v>
       </c>
-      <c r="D5" s="8"/>
-      <c r="E5" s="7">
+      <c r="D5" s="10"/>
+      <c r="E5" s="9">
         <v>34</v>
       </c>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8"/>
-      <c r="I5" s="8"/>
-      <c r="J5" s="8"/>
-      <c r="K5" s="7">
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="9">
         <v>2</v>
       </c>
-      <c r="L5" t="s" s="7">
+      <c r="I5" t="s" s="9">
         <v>26</v>
       </c>
-      <c r="M5" t="s" s="7">
+      <c r="J5" t="s" s="9">
         <v>27</v>
       </c>
-      <c r="N5" t="s" s="7">
+      <c r="K5" t="s" s="9">
         <v>28</v>
       </c>
-      <c r="O5" s="7">
+      <c r="L5" s="9">
         <v>1952</v>
       </c>
-      <c r="P5" t="s" s="7">
+      <c r="M5" t="s" s="9">
         <v>29</v>
       </c>
-      <c r="Q5" s="8"/>
-      <c r="R5" s="8"/>
-      <c r="S5" s="7">
+      <c r="N5" s="10"/>
+      <c r="O5" s="10"/>
+      <c r="P5" s="9">
         <v>14.4781851182943</v>
       </c>
-      <c r="T5" s="8"/>
-      <c r="U5" s="8"/>
-      <c r="V5" t="s" s="7">
+      <c r="Q5" s="10"/>
+      <c r="R5" s="10"/>
+      <c r="S5" t="s" s="9">
         <v>30</v>
       </c>
-      <c r="W5" s="8"/>
-      <c r="X5" s="8"/>
-      <c r="Y5" s="8"/>
-      <c r="Z5" t="s" s="7">
+      <c r="T5" s="10"/>
+      <c r="U5" s="10"/>
+      <c r="V5" s="10"/>
+      <c r="W5" t="s" s="9">
         <v>32</v>
       </c>
+      <c r="X5" s="11"/>
+      <c r="Y5" s="11"/>
+      <c r="Z5" s="11"/>
     </row>
     <row r="6" ht="20.35" customHeight="1">
-      <c r="A6" s="7">
+      <c r="A6" s="9">
         <v>165</v>
       </c>
-      <c r="B6" s="8"/>
-      <c r="C6" s="7">
+      <c r="B6" s="10"/>
+      <c r="C6" s="9">
         <v>686</v>
       </c>
-      <c r="D6" s="8"/>
-      <c r="E6" s="7">
+      <c r="D6" s="10"/>
+      <c r="E6" s="9">
         <v>34</v>
       </c>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
-      <c r="I6" s="8"/>
-      <c r="J6" s="8"/>
-      <c r="K6" s="7">
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="9">
         <v>2</v>
       </c>
-      <c r="L6" t="s" s="7">
+      <c r="I6" t="s" s="9">
         <v>26</v>
       </c>
-      <c r="M6" t="s" s="7">
+      <c r="J6" t="s" s="9">
         <v>27</v>
       </c>
-      <c r="N6" t="s" s="7">
+      <c r="K6" t="s" s="9">
         <v>28</v>
       </c>
-      <c r="O6" s="7">
+      <c r="L6" s="9">
         <v>1953</v>
       </c>
-      <c r="P6" t="s" s="7">
+      <c r="M6" t="s" s="9">
         <v>29</v>
       </c>
-      <c r="Q6" s="8"/>
-      <c r="R6" s="8"/>
-      <c r="S6" s="7">
+      <c r="N6" s="10"/>
+      <c r="O6" s="10"/>
+      <c r="P6" s="9">
         <v>114.736682010622</v>
       </c>
-      <c r="T6" s="8"/>
-      <c r="U6" s="8"/>
-      <c r="V6" t="s" s="7">
+      <c r="Q6" s="10"/>
+      <c r="R6" s="10"/>
+      <c r="S6" t="s" s="9">
         <v>30</v>
       </c>
-      <c r="W6" s="8"/>
-      <c r="X6" s="8"/>
-      <c r="Y6" s="8"/>
-      <c r="Z6" t="s" s="7">
+      <c r="T6" s="10"/>
+      <c r="U6" s="10"/>
+      <c r="V6" s="10"/>
+      <c r="W6" t="s" s="9">
         <v>31</v>
       </c>
+      <c r="X6" s="11"/>
+      <c r="Y6" s="11"/>
+      <c r="Z6" s="11"/>
     </row>
     <row r="7" ht="20.35" customHeight="1">
-      <c r="A7" s="7">
+      <c r="A7" s="9">
         <v>165</v>
       </c>
-      <c r="B7" s="8"/>
-      <c r="C7" s="7">
+      <c r="B7" s="10"/>
+      <c r="C7" s="9">
         <v>686</v>
       </c>
-      <c r="D7" s="8"/>
-      <c r="E7" s="7">
+      <c r="D7" s="10"/>
+      <c r="E7" s="9">
         <v>34</v>
       </c>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="8"/>
-      <c r="I7" s="8"/>
-      <c r="J7" s="8"/>
-      <c r="K7" s="7">
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="9">
         <v>2</v>
       </c>
-      <c r="L7" t="s" s="7">
+      <c r="I7" t="s" s="9">
         <v>26</v>
       </c>
-      <c r="M7" t="s" s="7">
+      <c r="J7" t="s" s="9">
         <v>27</v>
       </c>
-      <c r="N7" t="s" s="7">
+      <c r="K7" t="s" s="9">
         <v>28</v>
       </c>
-      <c r="O7" s="7">
+      <c r="L7" s="9">
         <v>1953</v>
       </c>
-      <c r="P7" t="s" s="7">
+      <c r="M7" t="s" s="9">
         <v>29</v>
       </c>
-      <c r="Q7" s="8"/>
-      <c r="R7" s="8"/>
-      <c r="S7" s="7">
+      <c r="N7" s="10"/>
+      <c r="O7" s="10"/>
+      <c r="P7" s="9">
         <v>21.7172776774415</v>
       </c>
-      <c r="T7" s="8"/>
-      <c r="U7" s="8"/>
-      <c r="V7" t="s" s="7">
+      <c r="Q7" s="10"/>
+      <c r="R7" s="10"/>
+      <c r="S7" t="s" s="9">
         <v>30</v>
       </c>
-      <c r="W7" s="8"/>
-      <c r="X7" s="8"/>
-      <c r="Y7" s="8"/>
-      <c r="Z7" t="s" s="7">
+      <c r="T7" s="10"/>
+      <c r="U7" s="10"/>
+      <c r="V7" s="10"/>
+      <c r="W7" t="s" s="9">
         <v>32</v>
       </c>
+      <c r="X7" s="11"/>
+      <c r="Y7" s="11"/>
+      <c r="Z7" s="11"/>
     </row>
     <row r="8" ht="20.35" customHeight="1">
-      <c r="A8" s="7">
+      <c r="A8" s="9">
         <v>165</v>
       </c>
-      <c r="B8" s="8"/>
-      <c r="C8" s="7">
+      <c r="B8" s="10"/>
+      <c r="C8" s="9">
         <v>686</v>
       </c>
-      <c r="D8" s="8"/>
-      <c r="E8" s="7">
+      <c r="D8" s="10"/>
+      <c r="E8" s="9">
         <v>34</v>
       </c>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8"/>
-      <c r="I8" s="8"/>
-      <c r="J8" s="8"/>
-      <c r="K8" s="7">
+      <c r="F8" s="10"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="9">
         <v>2</v>
       </c>
-      <c r="L8" t="s" s="7">
+      <c r="I8" t="s" s="9">
         <v>26</v>
       </c>
-      <c r="M8" t="s" s="7">
+      <c r="J8" t="s" s="9">
         <v>27</v>
       </c>
-      <c r="N8" t="s" s="7">
+      <c r="K8" t="s" s="9">
         <v>28</v>
       </c>
-      <c r="O8" s="7">
+      <c r="L8" s="9">
         <v>1954</v>
       </c>
-      <c r="P8" t="s" s="7">
+      <c r="M8" t="s" s="9">
         <v>29</v>
       </c>
-      <c r="Q8" s="8"/>
-      <c r="R8" s="8"/>
-      <c r="S8" s="7">
+      <c r="N8" s="10"/>
+      <c r="O8" s="10"/>
+      <c r="P8" s="9">
         <v>203.387341351136</v>
       </c>
-      <c r="T8" s="8"/>
-      <c r="U8" s="8"/>
-      <c r="V8" t="s" s="7">
+      <c r="Q8" s="10"/>
+      <c r="R8" s="10"/>
+      <c r="S8" t="s" s="9">
         <v>30</v>
       </c>
-      <c r="W8" s="8"/>
-      <c r="X8" s="8"/>
-      <c r="Y8" s="8"/>
-      <c r="Z8" t="s" s="7">
+      <c r="T8" s="10"/>
+      <c r="U8" s="10"/>
+      <c r="V8" s="10"/>
+      <c r="W8" t="s" s="9">
         <v>31</v>
       </c>
+      <c r="X8" s="11"/>
+      <c r="Y8" s="11"/>
+      <c r="Z8" s="11"/>
     </row>
     <row r="9" ht="20.35" customHeight="1">
-      <c r="A9" s="7">
+      <c r="A9" s="9">
         <v>165</v>
       </c>
-      <c r="B9" s="8"/>
-      <c r="C9" s="7">
+      <c r="B9" s="10"/>
+      <c r="C9" s="9">
         <v>686</v>
       </c>
-      <c r="D9" s="8"/>
-      <c r="E9" s="7">
+      <c r="D9" s="10"/>
+      <c r="E9" s="9">
         <v>34</v>
       </c>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
-      <c r="I9" s="8"/>
-      <c r="J9" s="8"/>
-      <c r="K9" s="7">
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="9">
         <v>2</v>
       </c>
-      <c r="L9" t="s" s="7">
+      <c r="I9" t="s" s="9">
         <v>26</v>
       </c>
-      <c r="M9" t="s" s="7">
+      <c r="J9" t="s" s="9">
         <v>27</v>
       </c>
-      <c r="N9" t="s" s="7">
+      <c r="K9" t="s" s="9">
         <v>28</v>
       </c>
-      <c r="O9" s="7">
+      <c r="L9" s="9">
         <v>1954</v>
       </c>
-      <c r="P9" t="s" s="7">
+      <c r="M9" t="s" s="9">
         <v>29</v>
       </c>
-      <c r="Q9" s="8"/>
-      <c r="R9" s="8"/>
-      <c r="S9" s="7">
+      <c r="N9" s="10"/>
+      <c r="O9" s="10"/>
+      <c r="P9" s="9">
         <v>28.9563702365887</v>
       </c>
-      <c r="T9" s="8"/>
-      <c r="U9" s="8"/>
-      <c r="V9" t="s" s="7">
+      <c r="Q9" s="10"/>
+      <c r="R9" s="10"/>
+      <c r="S9" t="s" s="9">
         <v>30</v>
       </c>
-      <c r="W9" s="8"/>
-      <c r="X9" s="8"/>
-      <c r="Y9" s="8"/>
-      <c r="Z9" t="s" s="7">
+      <c r="T9" s="10"/>
+      <c r="U9" s="10"/>
+      <c r="V9" s="10"/>
+      <c r="W9" t="s" s="9">
         <v>32</v>
       </c>
+      <c r="X9" s="11"/>
+      <c r="Y9" s="11"/>
+      <c r="Z9" s="11"/>
     </row>
     <row r="10" ht="20.35" customHeight="1">
-      <c r="A10" s="7">
+      <c r="A10" s="9">
         <v>165</v>
       </c>
-      <c r="B10" s="8"/>
-      <c r="C10" s="7">
+      <c r="B10" s="10"/>
+      <c r="C10" s="9">
         <v>686</v>
       </c>
-      <c r="D10" s="8"/>
-      <c r="E10" s="7">
+      <c r="D10" s="10"/>
+      <c r="E10" s="9">
         <v>34</v>
       </c>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8"/>
-      <c r="I10" s="8"/>
-      <c r="J10" s="8"/>
-      <c r="K10" s="7">
+      <c r="F10" s="10"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="9">
         <v>2</v>
       </c>
-      <c r="L10" t="s" s="7">
+      <c r="I10" t="s" s="9">
         <v>26</v>
       </c>
-      <c r="M10" t="s" s="7">
+      <c r="J10" t="s" s="9">
         <v>27</v>
       </c>
-      <c r="N10" t="s" s="7">
+      <c r="K10" t="s" s="9">
         <v>28</v>
       </c>
-      <c r="O10" s="7">
+      <c r="L10" s="9">
         <v>1955</v>
       </c>
-      <c r="P10" t="s" s="7">
+      <c r="M10" t="s" s="9">
         <v>29</v>
       </c>
-      <c r="Q10" s="8"/>
-      <c r="R10" s="8"/>
-      <c r="S10" s="7">
+      <c r="N10" s="10"/>
+      <c r="O10" s="10"/>
+      <c r="P10" s="9">
         <v>316.865073859446</v>
       </c>
-      <c r="T10" s="8"/>
-      <c r="U10" s="8"/>
-      <c r="V10" t="s" s="7">
+      <c r="Q10" s="10"/>
+      <c r="R10" s="10"/>
+      <c r="S10" t="s" s="9">
         <v>30</v>
       </c>
-      <c r="W10" s="8"/>
-      <c r="X10" s="8"/>
-      <c r="Y10" s="8"/>
-      <c r="Z10" t="s" s="7">
+      <c r="T10" s="10"/>
+      <c r="U10" s="10"/>
+      <c r="V10" s="10"/>
+      <c r="W10" t="s" s="9">
         <v>31</v>
       </c>
+      <c r="X10" s="11"/>
+      <c r="Y10" s="11"/>
+      <c r="Z10" s="11"/>
     </row>
     <row r="11" ht="20.35" customHeight="1">
-      <c r="A11" s="9"/>
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="8"/>
-      <c r="I11" s="8"/>
-      <c r="J11" s="8"/>
-      <c r="K11" s="8"/>
-      <c r="L11" s="8"/>
-      <c r="M11" s="8"/>
-      <c r="N11" s="8"/>
-      <c r="O11" s="8"/>
-      <c r="P11" s="8"/>
-      <c r="Q11" s="8"/>
-      <c r="R11" s="8"/>
-      <c r="S11" s="8"/>
-      <c r="T11" s="8"/>
-      <c r="U11" s="8"/>
-      <c r="V11" s="8"/>
-      <c r="W11" s="8"/>
-      <c r="X11" s="8"/>
-      <c r="Y11" s="8"/>
-      <c r="Z11" s="8"/>
+      <c r="A11" s="12"/>
+      <c r="B11" s="10"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="10"/>
+      <c r="I11" s="10"/>
+      <c r="J11" s="10"/>
+      <c r="K11" s="10"/>
+      <c r="L11" s="10"/>
+      <c r="M11" s="10"/>
+      <c r="N11" s="10"/>
+      <c r="O11" s="10"/>
+      <c r="P11" s="10"/>
+      <c r="Q11" s="10"/>
+      <c r="R11" s="10"/>
+      <c r="S11" s="10"/>
+      <c r="T11" s="10"/>
+      <c r="U11" s="10"/>
+      <c r="V11" s="10"/>
+      <c r="W11" s="10"/>
+      <c r="X11" s="10"/>
+      <c r="Y11" s="10"/>
+      <c r="Z11" s="10"/>
     </row>
     <row r="12" ht="20.35" customHeight="1">
-      <c r="A12" s="9"/>
-      <c r="B12" s="8"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="8"/>
-      <c r="I12" s="8"/>
-      <c r="J12" s="8"/>
-      <c r="K12" s="8"/>
-      <c r="L12" s="8"/>
-      <c r="M12" s="8"/>
-      <c r="N12" s="8"/>
-      <c r="O12" s="8"/>
-      <c r="P12" s="8"/>
-      <c r="Q12" s="8"/>
-      <c r="R12" s="8"/>
-      <c r="S12" s="8"/>
-      <c r="T12" s="8"/>
-      <c r="U12" s="8"/>
-      <c r="V12" s="8"/>
-      <c r="W12" s="8"/>
-      <c r="X12" s="8"/>
-      <c r="Y12" s="8"/>
-      <c r="Z12" s="8"/>
+      <c r="A12" s="12"/>
+      <c r="B12" s="10"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="10"/>
+      <c r="I12" s="10"/>
+      <c r="J12" s="10"/>
+      <c r="K12" s="10"/>
+      <c r="L12" s="10"/>
+      <c r="M12" s="10"/>
+      <c r="N12" s="10"/>
+      <c r="O12" s="10"/>
+      <c r="P12" s="10"/>
+      <c r="Q12" s="10"/>
+      <c r="R12" s="10"/>
+      <c r="S12" s="10"/>
+      <c r="T12" s="10"/>
+      <c r="U12" s="10"/>
+      <c r="V12" s="10"/>
+      <c r="W12" s="10"/>
+      <c r="X12" s="10"/>
+      <c r="Y12" s="10"/>
+      <c r="Z12" s="10"/>
     </row>
     <row r="13" ht="20.35" customHeight="1">
-      <c r="A13" s="9"/>
-      <c r="B13" s="8"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="8"/>
-      <c r="I13" s="8"/>
-      <c r="J13" s="8"/>
-      <c r="K13" s="8"/>
-      <c r="L13" s="8"/>
-      <c r="M13" s="8"/>
-      <c r="N13" s="8"/>
-      <c r="O13" s="8"/>
-      <c r="P13" s="8"/>
-      <c r="Q13" s="8"/>
-      <c r="R13" s="8"/>
-      <c r="S13" s="8"/>
-      <c r="T13" s="8"/>
-      <c r="U13" s="8"/>
-      <c r="V13" s="8"/>
-      <c r="W13" s="8"/>
-      <c r="X13" s="8"/>
-      <c r="Y13" s="8"/>
-      <c r="Z13" s="8"/>
+      <c r="A13" s="12"/>
+      <c r="B13" s="10"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="10"/>
+      <c r="I13" s="10"/>
+      <c r="J13" s="10"/>
+      <c r="K13" s="10"/>
+      <c r="L13" s="10"/>
+      <c r="M13" s="10"/>
+      <c r="N13" s="10"/>
+      <c r="O13" s="10"/>
+      <c r="P13" s="10"/>
+      <c r="Q13" s="10"/>
+      <c r="R13" s="10"/>
+      <c r="S13" s="10"/>
+      <c r="T13" s="10"/>
+      <c r="U13" s="10"/>
+      <c r="V13" s="10"/>
+      <c r="W13" s="10"/>
+      <c r="X13" s="10"/>
+      <c r="Y13" s="10"/>
+      <c r="Z13" s="10"/>
     </row>
     <row r="14" ht="20.35" customHeight="1">
-      <c r="A14" s="9"/>
-      <c r="B14" s="8"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="8"/>
-      <c r="H14" s="8"/>
-      <c r="I14" s="8"/>
-      <c r="J14" s="8"/>
-      <c r="K14" s="8"/>
-      <c r="L14" s="8"/>
-      <c r="M14" s="8"/>
-      <c r="N14" s="8"/>
-      <c r="O14" s="8"/>
-      <c r="P14" s="8"/>
-      <c r="Q14" s="8"/>
-      <c r="R14" s="8"/>
-      <c r="S14" s="8"/>
-      <c r="T14" s="8"/>
-      <c r="U14" s="8"/>
-      <c r="V14" s="8"/>
-      <c r="W14" s="8"/>
-      <c r="X14" s="8"/>
-      <c r="Y14" s="8"/>
-      <c r="Z14" s="8"/>
+      <c r="A14" s="12"/>
+      <c r="B14" s="10"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="10"/>
+      <c r="H14" s="10"/>
+      <c r="I14" s="10"/>
+      <c r="J14" s="10"/>
+      <c r="K14" s="10"/>
+      <c r="L14" s="10"/>
+      <c r="M14" s="10"/>
+      <c r="N14" s="10"/>
+      <c r="O14" s="10"/>
+      <c r="P14" s="10"/>
+      <c r="Q14" s="10"/>
+      <c r="R14" s="10"/>
+      <c r="S14" s="10"/>
+      <c r="T14" s="10"/>
+      <c r="U14" s="10"/>
+      <c r="V14" s="10"/>
+      <c r="W14" s="10"/>
+      <c r="X14" s="10"/>
+      <c r="Y14" s="10"/>
+      <c r="Z14" s="10"/>
     </row>
     <row r="15" ht="20.35" customHeight="1">
-      <c r="A15" s="9"/>
-      <c r="B15" s="8"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="8"/>
-      <c r="G15" s="8"/>
-      <c r="H15" s="8"/>
-      <c r="I15" s="8"/>
-      <c r="J15" s="8"/>
-      <c r="K15" s="8"/>
-      <c r="L15" s="8"/>
-      <c r="M15" s="8"/>
-      <c r="N15" s="8"/>
-      <c r="O15" s="8"/>
-      <c r="P15" s="8"/>
-      <c r="Q15" s="8"/>
-      <c r="R15" s="8"/>
-      <c r="S15" s="8"/>
-      <c r="T15" s="8"/>
-      <c r="U15" s="8"/>
-      <c r="V15" s="8"/>
-      <c r="W15" s="8"/>
-      <c r="X15" s="8"/>
-      <c r="Y15" s="8"/>
-      <c r="Z15" s="8"/>
+      <c r="A15" s="12"/>
+      <c r="B15" s="10"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="10"/>
+      <c r="H15" s="10"/>
+      <c r="I15" s="10"/>
+      <c r="J15" s="10"/>
+      <c r="K15" s="10"/>
+      <c r="L15" s="10"/>
+      <c r="M15" s="10"/>
+      <c r="N15" s="10"/>
+      <c r="O15" s="10"/>
+      <c r="P15" s="10"/>
+      <c r="Q15" s="10"/>
+      <c r="R15" s="10"/>
+      <c r="S15" s="10"/>
+      <c r="T15" s="10"/>
+      <c r="U15" s="10"/>
+      <c r="V15" s="10"/>
+      <c r="W15" s="10"/>
+      <c r="X15" s="10"/>
+      <c r="Y15" s="10"/>
+      <c r="Z15" s="10"/>
     </row>
     <row r="16" ht="20.35" customHeight="1">
-      <c r="A16" s="9"/>
-      <c r="B16" s="8"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="8"/>
-      <c r="G16" s="8"/>
-      <c r="H16" s="8"/>
-      <c r="I16" s="8"/>
-      <c r="J16" s="8"/>
-      <c r="K16" s="8"/>
-      <c r="L16" s="8"/>
-      <c r="M16" s="8"/>
-      <c r="N16" s="8"/>
-      <c r="O16" s="8"/>
-      <c r="P16" s="8"/>
-      <c r="Q16" s="8"/>
-      <c r="R16" s="8"/>
-      <c r="S16" s="8"/>
-      <c r="T16" s="8"/>
-      <c r="U16" s="8"/>
-      <c r="V16" s="8"/>
-      <c r="W16" s="8"/>
-      <c r="X16" s="8"/>
-      <c r="Y16" s="8"/>
-      <c r="Z16" s="8"/>
+      <c r="A16" s="12"/>
+      <c r="B16" s="10"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="10"/>
+      <c r="G16" s="10"/>
+      <c r="H16" s="10"/>
+      <c r="I16" s="10"/>
+      <c r="J16" s="10"/>
+      <c r="K16" s="10"/>
+      <c r="L16" s="10"/>
+      <c r="M16" s="10"/>
+      <c r="N16" s="10"/>
+      <c r="O16" s="10"/>
+      <c r="P16" s="10"/>
+      <c r="Q16" s="10"/>
+      <c r="R16" s="10"/>
+      <c r="S16" s="10"/>
+      <c r="T16" s="10"/>
+      <c r="U16" s="10"/>
+      <c r="V16" s="10"/>
+      <c r="W16" s="10"/>
+      <c r="X16" s="10"/>
+      <c r="Y16" s="10"/>
+      <c r="Z16" s="10"/>
     </row>
     <row r="17" ht="20.35" customHeight="1">
-      <c r="A17" s="9"/>
-      <c r="B17" s="8"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="8"/>
-      <c r="G17" s="8"/>
-      <c r="H17" s="8"/>
-      <c r="I17" s="8"/>
-      <c r="J17" s="8"/>
-      <c r="K17" s="8"/>
-      <c r="L17" s="8"/>
-      <c r="M17" s="8"/>
-      <c r="N17" s="8"/>
-      <c r="O17" s="8"/>
-      <c r="P17" s="8"/>
-      <c r="Q17" s="8"/>
-      <c r="R17" s="8"/>
-      <c r="S17" s="8"/>
-      <c r="T17" s="8"/>
-      <c r="U17" s="8"/>
-      <c r="V17" s="8"/>
-      <c r="W17" s="8"/>
-      <c r="X17" s="8"/>
-      <c r="Y17" s="8"/>
-      <c r="Z17" s="8"/>
+      <c r="A17" s="12"/>
+      <c r="B17" s="10"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="10"/>
+      <c r="G17" s="10"/>
+      <c r="H17" s="10"/>
+      <c r="I17" s="10"/>
+      <c r="J17" s="10"/>
+      <c r="K17" s="10"/>
+      <c r="L17" s="10"/>
+      <c r="M17" s="10"/>
+      <c r="N17" s="10"/>
+      <c r="O17" s="10"/>
+      <c r="P17" s="10"/>
+      <c r="Q17" s="10"/>
+      <c r="R17" s="10"/>
+      <c r="S17" s="10"/>
+      <c r="T17" s="10"/>
+      <c r="U17" s="10"/>
+      <c r="V17" s="10"/>
+      <c r="W17" s="10"/>
+      <c r="X17" s="10"/>
+      <c r="Y17" s="10"/>
+      <c r="Z17" s="10"/>
     </row>
     <row r="18" ht="20.35" customHeight="1">
-      <c r="A18" s="9"/>
-      <c r="B18" s="8"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
-      <c r="F18" s="8"/>
-      <c r="G18" s="8"/>
-      <c r="H18" s="8"/>
-      <c r="I18" s="8"/>
-      <c r="J18" s="8"/>
-      <c r="K18" s="8"/>
-      <c r="L18" s="8"/>
-      <c r="M18" s="8"/>
-      <c r="N18" s="8"/>
-      <c r="O18" s="8"/>
-      <c r="P18" s="8"/>
-      <c r="Q18" s="8"/>
-      <c r="R18" s="8"/>
-      <c r="S18" s="8"/>
-      <c r="T18" s="8"/>
-      <c r="U18" s="8"/>
-      <c r="V18" s="8"/>
-      <c r="W18" s="8"/>
-      <c r="X18" s="8"/>
-      <c r="Y18" s="8"/>
-      <c r="Z18" s="8"/>
+      <c r="A18" s="12"/>
+      <c r="B18" s="10"/>
+      <c r="C18" s="10"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="10"/>
+      <c r="G18" s="10"/>
+      <c r="H18" s="10"/>
+      <c r="I18" s="10"/>
+      <c r="J18" s="10"/>
+      <c r="K18" s="10"/>
+      <c r="L18" s="10"/>
+      <c r="M18" s="10"/>
+      <c r="N18" s="10"/>
+      <c r="O18" s="10"/>
+      <c r="P18" s="10"/>
+      <c r="Q18" s="10"/>
+      <c r="R18" s="10"/>
+      <c r="S18" s="10"/>
+      <c r="T18" s="10"/>
+      <c r="U18" s="10"/>
+      <c r="V18" s="10"/>
+      <c r="W18" s="10"/>
+      <c r="X18" s="10"/>
+      <c r="Y18" s="10"/>
+      <c r="Z18" s="10"/>
     </row>
     <row r="19" ht="20.35" customHeight="1">
-      <c r="A19" s="9"/>
-      <c r="B19" s="8"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="8"/>
-      <c r="G19" s="8"/>
-      <c r="H19" s="8"/>
-      <c r="I19" s="8"/>
-      <c r="J19" s="8"/>
-      <c r="K19" s="8"/>
-      <c r="L19" s="8"/>
-      <c r="M19" s="8"/>
-      <c r="N19" s="8"/>
-      <c r="O19" s="8"/>
-      <c r="P19" s="8"/>
-      <c r="Q19" s="8"/>
-      <c r="R19" s="8"/>
-      <c r="S19" s="8"/>
-      <c r="T19" s="8"/>
-      <c r="U19" s="8"/>
-      <c r="V19" s="8"/>
-      <c r="W19" s="8"/>
-      <c r="X19" s="8"/>
-      <c r="Y19" s="8"/>
-      <c r="Z19" s="8"/>
+      <c r="A19" s="12"/>
+      <c r="B19" s="10"/>
+      <c r="C19" s="10"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="10"/>
+      <c r="F19" s="10"/>
+      <c r="G19" s="10"/>
+      <c r="H19" s="10"/>
+      <c r="I19" s="10"/>
+      <c r="J19" s="10"/>
+      <c r="K19" s="10"/>
+      <c r="L19" s="10"/>
+      <c r="M19" s="10"/>
+      <c r="N19" s="10"/>
+      <c r="O19" s="10"/>
+      <c r="P19" s="10"/>
+      <c r="Q19" s="10"/>
+      <c r="R19" s="10"/>
+      <c r="S19" s="10"/>
+      <c r="T19" s="10"/>
+      <c r="U19" s="10"/>
+      <c r="V19" s="10"/>
+      <c r="W19" s="10"/>
+      <c r="X19" s="10"/>
+      <c r="Y19" s="10"/>
+      <c r="Z19" s="10"/>
     </row>
     <row r="20" ht="20.35" customHeight="1">
-      <c r="A20" s="9"/>
-      <c r="B20" s="8"/>
-      <c r="C20" s="8"/>
-      <c r="D20" s="8"/>
-      <c r="E20" s="8"/>
-      <c r="F20" s="8"/>
-      <c r="G20" s="8"/>
-      <c r="H20" s="8"/>
-      <c r="I20" s="8"/>
-      <c r="J20" s="8"/>
-      <c r="K20" s="8"/>
-      <c r="L20" s="8"/>
-      <c r="M20" s="8"/>
-      <c r="N20" s="8"/>
-      <c r="O20" s="8"/>
-      <c r="P20" s="8"/>
-      <c r="Q20" s="8"/>
-      <c r="R20" s="8"/>
-      <c r="S20" s="8"/>
-      <c r="T20" s="8"/>
-      <c r="U20" s="8"/>
-      <c r="V20" s="8"/>
-      <c r="W20" s="8"/>
-      <c r="X20" s="8"/>
-      <c r="Y20" s="8"/>
-      <c r="Z20" s="8"/>
+      <c r="A20" s="12"/>
+      <c r="B20" s="10"/>
+      <c r="C20" s="10"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="10"/>
+      <c r="F20" s="10"/>
+      <c r="G20" s="10"/>
+      <c r="H20" s="10"/>
+      <c r="I20" s="10"/>
+      <c r="J20" s="10"/>
+      <c r="K20" s="10"/>
+      <c r="L20" s="10"/>
+      <c r="M20" s="10"/>
+      <c r="N20" s="10"/>
+      <c r="O20" s="10"/>
+      <c r="P20" s="10"/>
+      <c r="Q20" s="10"/>
+      <c r="R20" s="10"/>
+      <c r="S20" s="10"/>
+      <c r="T20" s="10"/>
+      <c r="U20" s="10"/>
+      <c r="V20" s="10"/>
+      <c r="W20" s="10"/>
+      <c r="X20" s="10"/>
+      <c r="Y20" s="10"/>
+      <c r="Z20" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
update test data for new template
</commit_message>
<xml_diff>
--- a/test_uploads/new_test_data.xlsx
+++ b/test_uploads/new_test_data.xlsx
@@ -17,60 +17,60 @@
     <t>fishing entity</t>
   </si>
   <si>
+    <t>EEZ</t>
+  </si>
+  <si>
+    <t>FAO area</t>
+  </si>
+  <si>
+    <t>layer</t>
+  </si>
+  <si>
+    <t>sector</t>
+  </si>
+  <si>
+    <t>catch type</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>taxon name</t>
+  </si>
+  <si>
+    <t>amount</t>
+  </si>
+  <si>
+    <t>input type</t>
+  </si>
+  <si>
     <t xml:space="preserve">original country fishing </t>
   </si>
   <si>
-    <t>EEZ</t>
-  </si>
-  <si>
     <t>EEZ sub area</t>
   </si>
   <si>
-    <t>FAO area</t>
-  </si>
-  <si>
     <t>subregional area</t>
   </si>
   <si>
     <t>province state</t>
   </si>
   <si>
-    <t>layer</t>
-  </si>
-  <si>
-    <t>sector</t>
-  </si>
-  <si>
     <t>original sector</t>
   </si>
   <si>
-    <t>catch type</t>
-  </si>
-  <si>
-    <t>year</t>
-  </si>
-  <si>
-    <t>taxon name</t>
-  </si>
-  <si>
     <t>original taxon name</t>
   </si>
   <si>
     <t>original FAO name</t>
   </si>
   <si>
-    <t>amount</t>
-  </si>
-  <si>
     <t>adjustment factor</t>
   </si>
   <si>
     <t>gear type</t>
   </si>
   <si>
-    <t>input type</t>
-  </si>
-  <si>
     <t>forward carry rule</t>
   </si>
   <si>
@@ -95,16 +95,16 @@
     <t>Industrial</t>
   </si>
   <si>
+    <t>Discards</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Trichiurus lepturus</t>
+  </si>
+  <si>
+    <t>Reconstructed</t>
+  </si>
+  <si>
     <t>LS, C</t>
-  </si>
-  <si>
-    <t>Discards</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Trichiurus lepturus</t>
-  </si>
-  <si>
-    <t>Reconstructed</t>
   </si>
   <si>
     <t xml:space="preserve">Trawlers, legal; ; ; </t>
@@ -1679,44 +1679,44 @@
       <c r="A2" s="6">
         <v>165</v>
       </c>
-      <c r="B2" s="7"/>
+      <c r="B2" s="6">
+        <v>686</v>
+      </c>
       <c r="C2" s="6">
-        <v>686</v>
-      </c>
-      <c r="D2" s="7"/>
-      <c r="E2" s="6">
         <v>34</v>
       </c>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="6">
+      <c r="D2" s="6">
         <v>2</v>
       </c>
-      <c r="I2" t="s" s="6">
+      <c r="E2" t="s" s="6">
         <v>26</v>
       </c>
+      <c r="F2" t="s" s="6">
+        <v>27</v>
+      </c>
+      <c r="G2" s="6">
+        <v>1951</v>
+      </c>
+      <c r="H2" t="s" s="6">
+        <v>28</v>
+      </c>
+      <c r="I2" s="6">
+        <v>12.8212595279804</v>
+      </c>
       <c r="J2" t="s" s="6">
-        <v>27</v>
-      </c>
-      <c r="K2" t="s" s="6">
-        <v>28</v>
-      </c>
-      <c r="L2" s="6">
-        <v>1951</v>
-      </c>
-      <c r="M2" t="s" s="6">
         <v>29</v>
       </c>
+      <c r="K2" s="7"/>
+      <c r="L2" s="7"/>
+      <c r="M2" s="7"/>
       <c r="N2" s="7"/>
-      <c r="O2" s="7"/>
-      <c r="P2" s="6">
-        <v>12.8212595279804</v>
-      </c>
+      <c r="O2" t="s" s="6">
+        <v>30</v>
+      </c>
+      <c r="P2" s="7"/>
       <c r="Q2" s="7"/>
       <c r="R2" s="7"/>
-      <c r="S2" t="s" s="6">
-        <v>30</v>
-      </c>
+      <c r="S2" s="7"/>
       <c r="T2" s="7"/>
       <c r="U2" s="7"/>
       <c r="V2" s="7"/>
@@ -1731,44 +1731,44 @@
       <c r="A3" s="9">
         <v>165</v>
       </c>
-      <c r="B3" s="10"/>
+      <c r="B3" s="9">
+        <v>686</v>
+      </c>
       <c r="C3" s="9">
-        <v>686</v>
-      </c>
-      <c r="D3" s="10"/>
-      <c r="E3" s="9">
         <v>34</v>
       </c>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="9">
+      <c r="D3" s="9">
         <v>2</v>
       </c>
-      <c r="I3" t="s" s="9">
+      <c r="E3" t="s" s="9">
         <v>26</v>
       </c>
+      <c r="F3" t="s" s="9">
+        <v>27</v>
+      </c>
+      <c r="G3" s="9">
+        <v>1951</v>
+      </c>
+      <c r="H3" t="s" s="9">
+        <v>28</v>
+      </c>
+      <c r="I3" s="9">
+        <v>7.23909255914716</v>
+      </c>
       <c r="J3" t="s" s="9">
-        <v>27</v>
-      </c>
-      <c r="K3" t="s" s="9">
-        <v>28</v>
-      </c>
-      <c r="L3" s="9">
-        <v>1951</v>
-      </c>
-      <c r="M3" t="s" s="9">
         <v>29</v>
       </c>
+      <c r="K3" s="10"/>
+      <c r="L3" s="10"/>
+      <c r="M3" s="10"/>
       <c r="N3" s="10"/>
-      <c r="O3" s="10"/>
-      <c r="P3" s="9">
-        <v>7.23909255914716</v>
-      </c>
+      <c r="O3" t="s" s="9">
+        <v>30</v>
+      </c>
+      <c r="P3" s="10"/>
       <c r="Q3" s="10"/>
       <c r="R3" s="10"/>
-      <c r="S3" t="s" s="9">
-        <v>30</v>
-      </c>
+      <c r="S3" s="10"/>
       <c r="T3" s="10"/>
       <c r="U3" s="10"/>
       <c r="V3" s="10"/>
@@ -1783,44 +1783,44 @@
       <c r="A4" s="9">
         <v>165</v>
       </c>
-      <c r="B4" s="10"/>
+      <c r="B4" s="9">
+        <v>686</v>
+      </c>
       <c r="C4" s="9">
-        <v>686</v>
-      </c>
-      <c r="D4" s="10"/>
-      <c r="E4" s="9">
         <v>34</v>
       </c>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="9">
+      <c r="D4" s="9">
         <v>2</v>
       </c>
-      <c r="I4" t="s" s="9">
+      <c r="E4" t="s" s="9">
         <v>26</v>
       </c>
+      <c r="F4" t="s" s="9">
+        <v>27</v>
+      </c>
+      <c r="G4" s="9">
+        <v>1952</v>
+      </c>
+      <c r="H4" t="s" s="9">
+        <v>28</v>
+      </c>
+      <c r="I4" s="9">
+        <v>51.140148484989</v>
+      </c>
       <c r="J4" t="s" s="9">
-        <v>27</v>
-      </c>
-      <c r="K4" t="s" s="9">
-        <v>28</v>
-      </c>
-      <c r="L4" s="9">
-        <v>1952</v>
-      </c>
-      <c r="M4" t="s" s="9">
         <v>29</v>
       </c>
+      <c r="K4" s="10"/>
+      <c r="L4" s="10"/>
+      <c r="M4" s="10"/>
       <c r="N4" s="10"/>
-      <c r="O4" s="10"/>
-      <c r="P4" s="9">
-        <v>51.140148484989</v>
-      </c>
+      <c r="O4" t="s" s="9">
+        <v>30</v>
+      </c>
+      <c r="P4" s="10"/>
       <c r="Q4" s="10"/>
       <c r="R4" s="10"/>
-      <c r="S4" t="s" s="9">
-        <v>30</v>
-      </c>
+      <c r="S4" s="10"/>
       <c r="T4" s="10"/>
       <c r="U4" s="10"/>
       <c r="V4" s="10"/>
@@ -1835,44 +1835,44 @@
       <c r="A5" s="9">
         <v>165</v>
       </c>
-      <c r="B5" s="10"/>
+      <c r="B5" s="9">
+        <v>686</v>
+      </c>
       <c r="C5" s="9">
-        <v>686</v>
-      </c>
-      <c r="D5" s="10"/>
-      <c r="E5" s="9">
         <v>34</v>
       </c>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="9">
+      <c r="D5" s="9">
         <v>2</v>
       </c>
-      <c r="I5" t="s" s="9">
+      <c r="E5" t="s" s="9">
         <v>26</v>
       </c>
+      <c r="F5" t="s" s="9">
+        <v>27</v>
+      </c>
+      <c r="G5" s="9">
+        <v>1952</v>
+      </c>
+      <c r="H5" t="s" s="9">
+        <v>28</v>
+      </c>
+      <c r="I5" s="9">
+        <v>14.4781851182943</v>
+      </c>
       <c r="J5" t="s" s="9">
-        <v>27</v>
-      </c>
-      <c r="K5" t="s" s="9">
-        <v>28</v>
-      </c>
-      <c r="L5" s="9">
-        <v>1952</v>
-      </c>
-      <c r="M5" t="s" s="9">
         <v>29</v>
       </c>
+      <c r="K5" s="10"/>
+      <c r="L5" s="10"/>
+      <c r="M5" s="10"/>
       <c r="N5" s="10"/>
-      <c r="O5" s="10"/>
-      <c r="P5" s="9">
-        <v>14.4781851182943</v>
-      </c>
+      <c r="O5" t="s" s="9">
+        <v>30</v>
+      </c>
+      <c r="P5" s="10"/>
       <c r="Q5" s="10"/>
       <c r="R5" s="10"/>
-      <c r="S5" t="s" s="9">
-        <v>30</v>
-      </c>
+      <c r="S5" s="10"/>
       <c r="T5" s="10"/>
       <c r="U5" s="10"/>
       <c r="V5" s="10"/>
@@ -1887,44 +1887,44 @@
       <c r="A6" s="9">
         <v>165</v>
       </c>
-      <c r="B6" s="10"/>
+      <c r="B6" s="9">
+        <v>686</v>
+      </c>
       <c r="C6" s="9">
-        <v>686</v>
-      </c>
-      <c r="D6" s="10"/>
-      <c r="E6" s="9">
         <v>34</v>
       </c>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="9">
+      <c r="D6" s="9">
         <v>2</v>
       </c>
-      <c r="I6" t="s" s="9">
+      <c r="E6" t="s" s="9">
         <v>26</v>
       </c>
+      <c r="F6" t="s" s="9">
+        <v>27</v>
+      </c>
+      <c r="G6" s="9">
+        <v>1953</v>
+      </c>
+      <c r="H6" t="s" s="9">
+        <v>28</v>
+      </c>
+      <c r="I6" s="9">
+        <v>114.736682010622</v>
+      </c>
       <c r="J6" t="s" s="9">
-        <v>27</v>
-      </c>
-      <c r="K6" t="s" s="9">
-        <v>28</v>
-      </c>
-      <c r="L6" s="9">
-        <v>1953</v>
-      </c>
-      <c r="M6" t="s" s="9">
         <v>29</v>
       </c>
+      <c r="K6" s="10"/>
+      <c r="L6" s="10"/>
+      <c r="M6" s="10"/>
       <c r="N6" s="10"/>
-      <c r="O6" s="10"/>
-      <c r="P6" s="9">
-        <v>114.736682010622</v>
-      </c>
+      <c r="O6" t="s" s="9">
+        <v>30</v>
+      </c>
+      <c r="P6" s="10"/>
       <c r="Q6" s="10"/>
       <c r="R6" s="10"/>
-      <c r="S6" t="s" s="9">
-        <v>30</v>
-      </c>
+      <c r="S6" s="10"/>
       <c r="T6" s="10"/>
       <c r="U6" s="10"/>
       <c r="V6" s="10"/>
@@ -1939,44 +1939,44 @@
       <c r="A7" s="9">
         <v>165</v>
       </c>
-      <c r="B7" s="10"/>
+      <c r="B7" s="9">
+        <v>686</v>
+      </c>
       <c r="C7" s="9">
-        <v>686</v>
-      </c>
-      <c r="D7" s="10"/>
-      <c r="E7" s="9">
         <v>34</v>
       </c>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10"/>
-      <c r="H7" s="9">
+      <c r="D7" s="9">
         <v>2</v>
       </c>
-      <c r="I7" t="s" s="9">
+      <c r="E7" t="s" s="9">
         <v>26</v>
       </c>
+      <c r="F7" t="s" s="9">
+        <v>27</v>
+      </c>
+      <c r="G7" s="9">
+        <v>1953</v>
+      </c>
+      <c r="H7" t="s" s="9">
+        <v>28</v>
+      </c>
+      <c r="I7" s="9">
+        <v>21.7172776774415</v>
+      </c>
       <c r="J7" t="s" s="9">
-        <v>27</v>
-      </c>
-      <c r="K7" t="s" s="9">
-        <v>28</v>
-      </c>
-      <c r="L7" s="9">
-        <v>1953</v>
-      </c>
-      <c r="M7" t="s" s="9">
         <v>29</v>
       </c>
+      <c r="K7" s="10"/>
+      <c r="L7" s="10"/>
+      <c r="M7" s="10"/>
       <c r="N7" s="10"/>
-      <c r="O7" s="10"/>
-      <c r="P7" s="9">
-        <v>21.7172776774415</v>
-      </c>
+      <c r="O7" t="s" s="9">
+        <v>30</v>
+      </c>
+      <c r="P7" s="10"/>
       <c r="Q7" s="10"/>
       <c r="R7" s="10"/>
-      <c r="S7" t="s" s="9">
-        <v>30</v>
-      </c>
+      <c r="S7" s="10"/>
       <c r="T7" s="10"/>
       <c r="U7" s="10"/>
       <c r="V7" s="10"/>
@@ -1991,44 +1991,44 @@
       <c r="A8" s="9">
         <v>165</v>
       </c>
-      <c r="B8" s="10"/>
+      <c r="B8" s="9">
+        <v>686</v>
+      </c>
       <c r="C8" s="9">
-        <v>686</v>
-      </c>
-      <c r="D8" s="10"/>
-      <c r="E8" s="9">
         <v>34</v>
       </c>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="9">
+      <c r="D8" s="9">
         <v>2</v>
       </c>
-      <c r="I8" t="s" s="9">
+      <c r="E8" t="s" s="9">
         <v>26</v>
       </c>
+      <c r="F8" t="s" s="9">
+        <v>27</v>
+      </c>
+      <c r="G8" s="9">
+        <v>1954</v>
+      </c>
+      <c r="H8" t="s" s="9">
+        <v>28</v>
+      </c>
+      <c r="I8" s="9">
+        <v>203.387341351136</v>
+      </c>
       <c r="J8" t="s" s="9">
-        <v>27</v>
-      </c>
-      <c r="K8" t="s" s="9">
-        <v>28</v>
-      </c>
-      <c r="L8" s="9">
-        <v>1954</v>
-      </c>
-      <c r="M8" t="s" s="9">
         <v>29</v>
       </c>
+      <c r="K8" s="10"/>
+      <c r="L8" s="10"/>
+      <c r="M8" s="10"/>
       <c r="N8" s="10"/>
-      <c r="O8" s="10"/>
-      <c r="P8" s="9">
-        <v>203.387341351136</v>
-      </c>
+      <c r="O8" t="s" s="9">
+        <v>30</v>
+      </c>
+      <c r="P8" s="10"/>
       <c r="Q8" s="10"/>
       <c r="R8" s="10"/>
-      <c r="S8" t="s" s="9">
-        <v>30</v>
-      </c>
+      <c r="S8" s="10"/>
       <c r="T8" s="10"/>
       <c r="U8" s="10"/>
       <c r="V8" s="10"/>
@@ -2043,44 +2043,44 @@
       <c r="A9" s="9">
         <v>165</v>
       </c>
-      <c r="B9" s="10"/>
+      <c r="B9" s="9">
+        <v>686</v>
+      </c>
       <c r="C9" s="9">
-        <v>686</v>
-      </c>
-      <c r="D9" s="10"/>
-      <c r="E9" s="9">
         <v>34</v>
       </c>
-      <c r="F9" s="10"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="9">
+      <c r="D9" s="9">
         <v>2</v>
       </c>
-      <c r="I9" t="s" s="9">
+      <c r="E9" t="s" s="9">
         <v>26</v>
       </c>
+      <c r="F9" t="s" s="9">
+        <v>27</v>
+      </c>
+      <c r="G9" s="9">
+        <v>1954</v>
+      </c>
+      <c r="H9" t="s" s="9">
+        <v>28</v>
+      </c>
+      <c r="I9" s="9">
+        <v>28.9563702365887</v>
+      </c>
       <c r="J9" t="s" s="9">
-        <v>27</v>
-      </c>
-      <c r="K9" t="s" s="9">
-        <v>28</v>
-      </c>
-      <c r="L9" s="9">
-        <v>1954</v>
-      </c>
-      <c r="M9" t="s" s="9">
         <v>29</v>
       </c>
+      <c r="K9" s="10"/>
+      <c r="L9" s="10"/>
+      <c r="M9" s="10"/>
       <c r="N9" s="10"/>
-      <c r="O9" s="10"/>
-      <c r="P9" s="9">
-        <v>28.9563702365887</v>
-      </c>
+      <c r="O9" t="s" s="9">
+        <v>30</v>
+      </c>
+      <c r="P9" s="10"/>
       <c r="Q9" s="10"/>
       <c r="R9" s="10"/>
-      <c r="S9" t="s" s="9">
-        <v>30</v>
-      </c>
+      <c r="S9" s="10"/>
       <c r="T9" s="10"/>
       <c r="U9" s="10"/>
       <c r="V9" s="10"/>
@@ -2095,44 +2095,44 @@
       <c r="A10" s="9">
         <v>165</v>
       </c>
-      <c r="B10" s="10"/>
+      <c r="B10" s="9">
+        <v>686</v>
+      </c>
       <c r="C10" s="9">
-        <v>686</v>
-      </c>
-      <c r="D10" s="10"/>
-      <c r="E10" s="9">
         <v>34</v>
       </c>
-      <c r="F10" s="10"/>
-      <c r="G10" s="10"/>
-      <c r="H10" s="9">
+      <c r="D10" s="9">
         <v>2</v>
       </c>
-      <c r="I10" t="s" s="9">
+      <c r="E10" t="s" s="9">
         <v>26</v>
       </c>
+      <c r="F10" t="s" s="9">
+        <v>27</v>
+      </c>
+      <c r="G10" s="9">
+        <v>1955</v>
+      </c>
+      <c r="H10" t="s" s="9">
+        <v>28</v>
+      </c>
+      <c r="I10" s="9">
+        <v>316.865073859446</v>
+      </c>
       <c r="J10" t="s" s="9">
-        <v>27</v>
-      </c>
-      <c r="K10" t="s" s="9">
-        <v>28</v>
-      </c>
-      <c r="L10" s="9">
-        <v>1955</v>
-      </c>
-      <c r="M10" t="s" s="9">
         <v>29</v>
       </c>
+      <c r="K10" s="10"/>
+      <c r="L10" s="10"/>
+      <c r="M10" s="10"/>
       <c r="N10" s="10"/>
-      <c r="O10" s="10"/>
-      <c r="P10" s="9">
-        <v>316.865073859446</v>
-      </c>
+      <c r="O10" t="s" s="9">
+        <v>30</v>
+      </c>
+      <c r="P10" s="10"/>
       <c r="Q10" s="10"/>
       <c r="R10" s="10"/>
-      <c r="S10" t="s" s="9">
-        <v>30</v>
-      </c>
+      <c r="S10" s="10"/>
       <c r="T10" s="10"/>
       <c r="U10" s="10"/>
       <c r="V10" s="10"/>

</xml_diff>